<commit_message>
refactor: small changes in test_scenario document
</commit_message>
<xml_diff>
--- a/Test_Plan-Test_Cases/Test_Scenarios.xlsx
+++ b/Test_Plan-Test_Cases/Test_Scenarios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subed\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA Study\test-assessment\Test_Plan-Test_Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02136547-CC24-4E2C-AA98-36A7F8CA003F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CFCE3B-C187-44A6-8EF5-66A9C4F17659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E8" sqref="E8:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -589,7 +589,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -625,7 +625,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F10" s="2"/>
     </row>

</xml_diff>